<commit_message>
Update MCEE algorithm pseudocode
</commit_message>
<xml_diff>
--- a/docs/experiments/experiments.xlsx
+++ b/docs/experiments/experiments.xlsx
@@ -23,13 +23,13 @@
     <t>Linux 5.15.7-arch1-1</t>
   </si>
   <si>
-    <t>RRW = Round Robin Weighted</t>
+    <t>PoTC = Power of Two Choices</t>
   </si>
   <si>
     <t>Intel(R) Core(TM) i7-8700 CPU @ 3.20GHz 6 cores (2 threads per core) (mitigations off)</t>
   </si>
   <si>
-    <t>PoTC = Power of Two Choices</t>
+    <t>ES = Exact Search</t>
   </si>
   <si>
     <t xml:space="preserve">32 GB RAM </t>
@@ -41,7 +41,7 @@
     <t>Xms = 128MB, Xmx = 1024MB</t>
   </si>
   <si>
-    <t>MMDE = Maximal Matches Disjoint Enumeration</t>
+    <t>MCEE = Maximal Complex Event Enumeration (aka MMDE)</t>
   </si>
   <si>
     <t>mean</t>
@@ -101,13 +101,13 @@
     <t>DCERE(PoTC)</t>
   </si>
   <si>
-    <t>DCERE(RRW)</t>
+    <t>DCERE(ES)</t>
   </si>
   <si>
     <t>DCERE(MME)</t>
   </si>
   <si>
-    <t>DCERE(MMDE)</t>
+    <t>DCERE(MCEE)</t>
   </si>
   <si>
     <t>CORE2</t>
@@ -856,11 +856,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1923396158"/>
-        <c:axId val="1591371962"/>
+        <c:axId val="934261331"/>
+        <c:axId val="1679771806"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1923396158"/>
+        <c:axId val="934261331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,10 +912,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1591371962"/>
+        <c:crossAx val="1679771806"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1591371962"/>
+        <c:axId val="1679771806"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +990,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1923396158"/>
+        <c:crossAx val="934261331"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1106,11 +1106,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="995113550"/>
-        <c:axId val="548690712"/>
+        <c:axId val="634762073"/>
+        <c:axId val="1348585286"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="995113550"/>
+        <c:axId val="634762073"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,10 +1162,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="548690712"/>
+        <c:crossAx val="1348585286"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="548690712"/>
+        <c:axId val="1348585286"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,7 +1240,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="995113550"/>
+        <c:crossAx val="634762073"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1481,11 +1481,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1240641823"/>
-        <c:axId val="1957417495"/>
+        <c:axId val="1546850081"/>
+        <c:axId val="126348954"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1240641823"/>
+        <c:axId val="1546850081"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,10 +1537,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1957417495"/>
+        <c:crossAx val="126348954"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1957417495"/>
+        <c:axId val="126348954"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1615,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1240641823"/>
+        <c:crossAx val="1546850081"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1856,11 +1856,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1727428036"/>
-        <c:axId val="1911283271"/>
+        <c:axId val="1977526945"/>
+        <c:axId val="630044500"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1727428036"/>
+        <c:axId val="1977526945"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,10 +1912,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1911283271"/>
+        <c:crossAx val="630044500"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1911283271"/>
+        <c:axId val="630044500"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,7 +1990,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1727428036"/>
+        <c:crossAx val="1977526945"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2106,11 +2106,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="328146477"/>
-        <c:axId val="1459127135"/>
+        <c:axId val="828499067"/>
+        <c:axId val="1922110979"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="328146477"/>
+        <c:axId val="828499067"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2162,10 +2162,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1459127135"/>
+        <c:crossAx val="1922110979"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1459127135"/>
+        <c:axId val="1922110979"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2240,7 +2240,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328146477"/>
+        <c:crossAx val="828499067"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2356,11 +2356,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2072422656"/>
-        <c:axId val="1837751763"/>
+        <c:axId val="1106906245"/>
+        <c:axId val="1283657527"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2072422656"/>
+        <c:axId val="1106906245"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2412,10 +2412,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1837751763"/>
+        <c:crossAx val="1283657527"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1837751763"/>
+        <c:axId val="1283657527"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2490,7 +2490,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2072422656"/>
+        <c:crossAx val="1106906245"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2606,11 +2606,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="826700132"/>
-        <c:axId val="502799725"/>
+        <c:axId val="239656646"/>
+        <c:axId val="1594355953"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="826700132"/>
+        <c:axId val="239656646"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2662,10 +2662,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="502799725"/>
+        <c:crossAx val="1594355953"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="502799725"/>
+        <c:axId val="1594355953"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2740,7 +2740,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="826700132"/>
+        <c:crossAx val="239656646"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2857,11 +2857,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="56361392"/>
-        <c:axId val="1837927965"/>
+        <c:axId val="1665666564"/>
+        <c:axId val="1707669743"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="56361392"/>
+        <c:axId val="1665666564"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2913,10 +2913,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1837927965"/>
+        <c:crossAx val="1707669743"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1837927965"/>
+        <c:axId val="1707669743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2991,7 +2991,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56361392"/>
+        <c:crossAx val="1665666564"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -3207,11 +3207,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="461883441"/>
-        <c:axId val="346820849"/>
+        <c:axId val="1588567133"/>
+        <c:axId val="1913540743"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="461883441"/>
+        <c:axId val="1588567133"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3263,10 +3263,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346820849"/>
+        <c:crossAx val="1913540743"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="346820849"/>
+        <c:axId val="1913540743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3341,7 +3341,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="461883441"/>
+        <c:crossAx val="1588567133"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3582,11 +3582,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2017643718"/>
-        <c:axId val="1319329108"/>
+        <c:axId val="57371127"/>
+        <c:axId val="1884418578"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2017643718"/>
+        <c:axId val="57371127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3638,10 +3638,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1319329108"/>
+        <c:crossAx val="1884418578"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1319329108"/>
+        <c:axId val="1884418578"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3716,7 +3716,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2017643718"/>
+        <c:crossAx val="57371127"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3931,11 +3931,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="320843300"/>
-        <c:axId val="782861197"/>
+        <c:axId val="1906560915"/>
+        <c:axId val="1862824619"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="320843300"/>
+        <c:axId val="1906560915"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3987,10 +3987,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="782861197"/>
+        <c:crossAx val="1862824619"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="782861197"/>
+        <c:axId val="1862824619"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4065,7 +4065,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320843300"/>
+        <c:crossAx val="1906560915"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4306,11 +4306,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2059164435"/>
-        <c:axId val="148093263"/>
+        <c:axId val="71917208"/>
+        <c:axId val="466861547"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2059164435"/>
+        <c:axId val="71917208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4362,10 +4362,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="148093263"/>
+        <c:crossAx val="466861547"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148093263"/>
+        <c:axId val="466861547"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4440,7 +4440,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2059164435"/>
+        <c:crossAx val="71917208"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4655,11 +4655,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1451388832"/>
-        <c:axId val="1380582462"/>
+        <c:axId val="639766396"/>
+        <c:axId val="1826117565"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1451388832"/>
+        <c:axId val="639766396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4711,10 +4711,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1380582462"/>
+        <c:crossAx val="1826117565"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1380582462"/>
+        <c:axId val="1826117565"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4789,7 +4789,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1451388832"/>
+        <c:crossAx val="639766396"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5004,11 +5004,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1298003417"/>
-        <c:axId val="2004684326"/>
+        <c:axId val="1697344573"/>
+        <c:axId val="1250018582"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1298003417"/>
+        <c:axId val="1697344573"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -5061,10 +5061,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2004684326"/>
+        <c:crossAx val="1250018582"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2004684326"/>
+        <c:axId val="1250018582"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5139,7 +5139,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1298003417"/>
+        <c:crossAx val="1697344573"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5354,11 +5354,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="618124410"/>
-        <c:axId val="2093522440"/>
+        <c:axId val="1330192525"/>
+        <c:axId val="1211828591"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="618124410"/>
+        <c:axId val="1330192525"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -5411,10 +5411,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2093522440"/>
+        <c:crossAx val="1211828591"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2093522440"/>
+        <c:axId val="1211828591"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5489,7 +5489,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="618124410"/>
+        <c:crossAx val="1330192525"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5730,11 +5730,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1853408514"/>
-        <c:axId val="106500839"/>
+        <c:axId val="528628331"/>
+        <c:axId val="2071520665"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1853408514"/>
+        <c:axId val="528628331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5786,10 +5786,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106500839"/>
+        <c:crossAx val="2071520665"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106500839"/>
+        <c:axId val="2071520665"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5864,7 +5864,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1853408514"/>
+        <c:crossAx val="528628331"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -8311,9 +8311,9 @@
     <mergeCell ref="S23:W23"/>
     <mergeCell ref="T24:W24"/>
     <mergeCell ref="T34:W34"/>
-    <mergeCell ref="M44:Q44"/>
     <mergeCell ref="S42:W42"/>
     <mergeCell ref="S43:W43"/>
+    <mergeCell ref="M44:Q44"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H10:K10"/>

</xml_diff>